<commit_message>
Beginning work on game simulation, moved Awareness to Defense.
</commit_message>
<xml_diff>
--- a/plans/stats wiggler.xlsx
+++ b/plans/stats wiggler.xlsx
@@ -737,7 +737,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="R2" s="13">
         <f t="array" aca="1" ref="R2" ca="1">SUM(IF(attribs=R1,adjusted,0))</f>
-        <v>2.3119047619047617</v>
+        <v>2.3785714285714286</v>
       </c>
       <c r="S2" s="13">
         <f t="array" aca="1" ref="S2" ca="1">SUM(IF(attribs=S1,adjusted,0))</f>
@@ -816,11 +816,11 @@
       </c>
       <c r="T2" s="13">
         <f t="array" aca="1" ref="T2" ca="1">SUM(IF(attribs=T1,adjusted,0))</f>
-        <v>2.5785714285714287</v>
+        <v>2.611904761904762</v>
       </c>
       <c r="U2" s="13">
         <f t="array" aca="1" ref="U2" ca="1">SUM(IF(attribs=U1,adjusted,0))</f>
-        <v>2.6785714285714284</v>
+        <v>2.5785714285714283</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="str">
-        <f t="shared" ref="F3:F31" si="0">IF(ISBLANK(E3), "",
+        <f>IF(ISBLANK(E3), "",
     INDEX(attribs, MATCH(E3,ratings,0))=D3
 )</f>
         <v/>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H31" ca="1" si="1">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
+        <f t="shared" ref="H3:H31" ca="1" si="0">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
 I3/
 SUM(OFFSET(
     weights,
@@ -914,7 +914,9 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E4), "",
+    INDEX(attribs, MATCH(E4,ratings,0))=D4
+)</f>
         <v/>
       </c>
       <c r="G4" s="5">
@@ -922,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.8</v>
       </c>
       <c r="I4" s="6">
@@ -979,7 +981,9 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E5), "",
+    INDEX(attribs, MATCH(E5,ratings,0))=D5
+)</f>
         <v/>
       </c>
       <c r="G5" s="5">
@@ -987,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.4</v>
       </c>
       <c r="I5" s="6">
@@ -1046,7 +1050,9 @@
         <v>18</v>
       </c>
       <c r="F6" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E6), "",
+    INDEX(attribs, MATCH(E6,ratings,0))=D6
+)</f>
         <v>1</v>
       </c>
       <c r="G6" s="8">
@@ -1054,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="I6" s="9">
@@ -1117,7 +1123,9 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E7), "",
+    INDEX(attribs, MATCH(E7,ratings,0))=D7
+)</f>
         <v>1</v>
       </c>
       <c r="G7" s="2">
@@ -1125,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I7" s="3">
@@ -1182,7 +1190,9 @@
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E8), "",
+    INDEX(attribs, MATCH(E8,ratings,0))=D8
+)</f>
         <v/>
       </c>
       <c r="G8" s="5">
@@ -1190,7 +1200,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I8" s="6">
@@ -1249,7 +1259,9 @@
         <v>23</v>
       </c>
       <c r="F9" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E9), "",
+    INDEX(attribs, MATCH(E9,ratings,0))=D9
+)</f>
         <v>1</v>
       </c>
       <c r="G9" s="8">
@@ -1257,7 +1269,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I9" s="9">
@@ -1320,7 +1332,9 @@
         <v>54</v>
       </c>
       <c r="F10" s="2" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E10), "",
+    INDEX(attribs, MATCH(E10,ratings,0))=D10
+)</f>
         <v>1</v>
       </c>
       <c r="G10" s="2">
@@ -1328,7 +1342,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I10" s="3">
@@ -1367,7 +1381,9 @@
         <v>13</v>
       </c>
       <c r="F11" s="5" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E11), "",
+    INDEX(attribs, MATCH(E11,ratings,0))=D11
+)</f>
         <v>1</v>
       </c>
       <c r="G11" s="5">
@@ -1375,7 +1391,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I11" s="6">
@@ -1411,7 +1427,9 @@
         <v>22</v>
       </c>
       <c r="F12" s="5" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E12), "",
+    INDEX(attribs, MATCH(E12,ratings,0))=D12
+)</f>
         <v>1</v>
       </c>
       <c r="G12" s="5">
@@ -1419,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I12" s="6">
@@ -1455,7 +1473,9 @@
         <v>5</v>
       </c>
       <c r="F13" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E13), "",
+    INDEX(attribs, MATCH(E13,ratings,0))=D13
+)</f>
         <v>1</v>
       </c>
       <c r="G13" s="8">
@@ -1463,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="I13" s="9">
@@ -1501,7 +1521,9 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E14), "",
+    INDEX(attribs, MATCH(E14,ratings,0))=D14
+)</f>
         <v/>
       </c>
       <c r="G14" s="2">
@@ -1509,8 +1531,8 @@
         <v>4</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I14" s="3">
         <v>2</v>
@@ -1543,7 +1565,9 @@
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E15), "",
+    INDEX(attribs, MATCH(E15,ratings,0))=D15
+)</f>
         <v/>
       </c>
       <c r="G15" s="5">
@@ -1551,8 +1575,8 @@
         <v>4</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="I15" s="6">
         <v>1.5</v>
@@ -1587,7 +1611,9 @@
         <v>17</v>
       </c>
       <c r="F16" s="5" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E16), "",
+    INDEX(attribs, MATCH(E16,ratings,0))=D16
+)</f>
         <v>1</v>
       </c>
       <c r="G16" s="5">
@@ -1595,8 +1621,8 @@
         <v>4</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
@@ -1631,7 +1657,9 @@
         <v>14</v>
       </c>
       <c r="F17" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E17), "",
+    INDEX(attribs, MATCH(E17,ratings,0))=D17
+)</f>
         <v>1</v>
       </c>
       <c r="G17" s="8">
@@ -1639,12 +1667,10 @@
         <v>4</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.15</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0.5</v>
-      </c>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="9"/>
       <c r="R17" s="11" t="str">
         <f t="array" ref="R17">IFERROR(INDEX(ratings,SMALL(IF(attribs=R$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(R$2))), "")</f>
         <v/>
@@ -1679,7 +1705,9 @@
         <v>57</v>
       </c>
       <c r="F18" s="2" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E18), "",
+    INDEX(attribs, MATCH(E18,ratings,0))=D18
+)</f>
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -1687,7 +1715,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.25</v>
       </c>
       <c r="I18" s="3">
@@ -1717,7 +1745,9 @@
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E19), "",
+    INDEX(attribs, MATCH(E19,ratings,0))=D19
+)</f>
         <v/>
       </c>
       <c r="G19" s="5">
@@ -1725,7 +1755,7 @@
         <v>5</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.25</v>
       </c>
       <c r="I19" s="6">
@@ -1759,7 +1789,9 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E20), "",
+    INDEX(attribs, MATCH(E20,ratings,0))=D20
+)</f>
         <v/>
       </c>
       <c r="G20" s="5">
@@ -1767,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.25</v>
       </c>
       <c r="I20" s="6">
@@ -1801,7 +1833,9 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E21), "",
+    INDEX(attribs, MATCH(E21,ratings,0))=D21
+)</f>
         <v/>
       </c>
       <c r="G21" s="8">
@@ -1809,7 +1843,7 @@
         <v>5</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.25</v>
       </c>
       <c r="I21" s="9">
@@ -1847,7 +1881,9 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E22), "",
+    INDEX(attribs, MATCH(E22,ratings,0))=D22
+)</f>
         <v/>
       </c>
       <c r="G22" s="2">
@@ -1855,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="I22" s="3">
@@ -1889,7 +1925,9 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E23), "",
+    INDEX(attribs, MATCH(E23,ratings,0))=D23
+)</f>
         <v/>
       </c>
       <c r="G23" s="5">
@@ -1897,7 +1935,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="I23" s="6">
@@ -1915,7 +1953,9 @@
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E24), "",
+    INDEX(attribs, MATCH(E24,ratings,0))=D24
+)</f>
         <v/>
       </c>
       <c r="G24" s="5">
@@ -1923,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="I24" s="6">
@@ -1941,7 +1981,9 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E25), "",
+    INDEX(attribs, MATCH(E25,ratings,0))=D25
+)</f>
         <v/>
       </c>
       <c r="G25" s="5">
@@ -1949,7 +1991,7 @@
         <v>6</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="I25" s="6">
@@ -1963,7 +2005,9 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E26), "",
+    INDEX(attribs, MATCH(E26,ratings,0))=D26
+)</f>
         <v/>
       </c>
       <c r="G26" s="8">
@@ -1971,7 +2015,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="I26" s="9">
@@ -1993,7 +2037,9 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E27), "",
+    INDEX(attribs, MATCH(E27,ratings,0))=D27
+)</f>
         <v/>
       </c>
       <c r="G27" s="2">
@@ -2001,7 +2047,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I27" s="3">
@@ -2019,7 +2065,9 @@
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E28), "",
+    INDEX(attribs, MATCH(E28,ratings,0))=D28
+)</f>
         <v/>
       </c>
       <c r="G28" s="5">
@@ -2027,7 +2075,7 @@
         <v>7</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I28" s="6">
@@ -2045,7 +2093,9 @@
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E29), "",
+    INDEX(attribs, MATCH(E29,ratings,0))=D29
+)</f>
         <v/>
       </c>
       <c r="G29" s="5">
@@ -2053,7 +2103,7 @@
         <v>7</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I29" s="6">
@@ -2071,7 +2121,9 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E30), "",
+    INDEX(attribs, MATCH(E30,ratings,0))=D30
+)</f>
         <v/>
       </c>
       <c r="G30" s="5">
@@ -2079,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I30" s="6">
@@ -2093,7 +2145,9 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(E31), "",
+    INDEX(attribs, MATCH(E31,ratings,0))=D31
+)</f>
         <v/>
       </c>
       <c r="G31" s="8">
@@ -2101,7 +2155,7 @@
         <v>7</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="I31" s="9">

</xml_diff>

<commit_message>
committing based on what was left
</commit_message>
<xml_diff>
--- a/plans/stats wiggler.xlsx
+++ b/plans/stats wiggler.xlsx
@@ -526,31 +526,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="7" tint="-0.24994659260841701"/>
@@ -860,7 +836,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="D16" sqref="C16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,7 +1511,7 @@
         <v>87</v>
       </c>
       <c r="Y9">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X9,ratings,0)), INDEX(adjusted,MATCH(LEFT(X9, FIND("/", X9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X9, LEN(X9) - FIND("/", X9)),ratings,0)))</f>
+        <f t="shared" ref="Y9:Y16" ca="1" si="2">IFERROR(INDEX(adjusted,MATCH(X9,ratings,0)), INDEX(adjusted,MATCH(LEFT(X9, FIND("/", X9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X9, LEN(X9) - FIND("/", X9)),ratings,0)))</f>
         <v>0.7</v>
       </c>
       <c r="Z9" t="s">
@@ -1545,7 +1521,7 @@
         <v>78</v>
       </c>
       <c r="AB9">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA9,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA9, FIND("/", AA9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA9, LEN(AA9) - FIND("/", AA9)),ratings,0)))</f>
+        <f t="shared" ref="AB9:AB20" ca="1" si="3">IFERROR(INDEX(adjusted,MATCH(AA9,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA9, FIND("/", AA9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA9, LEN(AA9) - FIND("/", AA9)),ratings,0)))</f>
         <v>0.53333333333333333</v>
       </c>
     </row>
@@ -1606,7 +1582,7 @@
         <v>69</v>
       </c>
       <c r="Y10">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X10,ratings,0)), INDEX(adjusted,MATCH(LEFT(X10, FIND("/", X10)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X10, LEN(X10) - FIND("/", X10)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Z10" t="s">
@@ -1616,7 +1592,7 @@
         <v>77</v>
       </c>
       <c r="AB10">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA10,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA10, FIND("/", AA10)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA10, LEN(AA10) - FIND("/", AA10)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -1633,7 +1609,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="5" t="b">
-        <f t="shared" ref="F11" si="2">IF(ISBLANK(E11), "",
+        <f t="shared" ref="F11" si="4">IF(ISBLANK(E11), "",
     INDEX(attribs, MATCH(E11,ratings,0))=D11
 )</f>
         <v>1</v>
@@ -1643,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ref="H11" ca="1" si="3">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
+        <f t="shared" ref="H11" ca="1" si="5">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
 I11/
 SUM(OFFSET(
     weights,
@@ -1680,7 +1656,7 @@
         <v>70</v>
       </c>
       <c r="Y11">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X11,ratings,0)), INDEX(adjusted,MATCH(LEFT(X11, FIND("/", X11)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X11, LEN(X11) - FIND("/", X11)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Z11" t="s">
@@ -1690,7 +1666,7 @@
         <v>69</v>
       </c>
       <c r="AB11">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA11,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA11, FIND("/", AA11)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA11, LEN(AA11) - FIND("/", AA11)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -1742,7 +1718,7 @@
         <v>88</v>
       </c>
       <c r="Y12">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X12,ratings,0)), INDEX(adjusted,MATCH(LEFT(X12, FIND("/", X12)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X12, LEN(X12) - FIND("/", X12)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Z12" t="s">
@@ -1752,7 +1728,7 @@
         <v>70</v>
       </c>
       <c r="AB12">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA12,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA12, FIND("/", AA12)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA12, LEN(AA12) - FIND("/", AA12)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -1806,7 +1782,7 @@
         <v>89</v>
       </c>
       <c r="Y13">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X13,ratings,0)), INDEX(adjusted,MATCH(LEFT(X13, FIND("/", X13)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X13, LEN(X13) - FIND("/", X13)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="Z13" t="s">
@@ -1816,7 +1792,7 @@
         <v>79</v>
       </c>
       <c r="AB13">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA13,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA13, FIND("/", AA13)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA13, LEN(AA13) - FIND("/", AA13)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1868,7 +1844,7 @@
         <v>71</v>
       </c>
       <c r="Y14">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X14,ratings,0)), INDEX(adjusted,MATCH(LEFT(X14, FIND("/", X14)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X14, LEN(X14) - FIND("/", X14)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.6333333333333333</v>
       </c>
       <c r="Z14" t="s">
@@ -1878,7 +1854,7 @@
         <v>80</v>
       </c>
       <c r="AB14">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA14,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA14, FIND("/", AA14)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA14, LEN(AA14) - FIND("/", AA14)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1934,7 +1910,7 @@
         <v>90</v>
       </c>
       <c r="Y15">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X15,ratings,0)), INDEX(adjusted,MATCH(LEFT(X15, FIND("/", X15)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X15, LEN(X15) - FIND("/", X15)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.76666666666666661</v>
       </c>
       <c r="Z15" t="s">
@@ -1944,7 +1920,7 @@
         <v>81</v>
       </c>
       <c r="AB15">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA15,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA15, FIND("/", AA15)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA15, LEN(AA15) - FIND("/", AA15)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.4</v>
       </c>
     </row>
@@ -1996,7 +1972,7 @@
         <v>85</v>
       </c>
       <c r="Y16">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(X16,ratings,0)), INDEX(adjusted,MATCH(LEFT(X16, FIND("/", X16)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X16, LEN(X16) - FIND("/", X16)),ratings,0)))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.48333333333333328</v>
       </c>
       <c r="Z16" t="s">
@@ -2006,7 +1982,7 @@
         <v>82</v>
       </c>
       <c r="AB16">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA16,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA16, FIND("/", AA16)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA16, LEN(AA16) - FIND("/", AA16)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2060,7 +2036,7 @@
         <v>71</v>
       </c>
       <c r="AB17">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA17,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA17, FIND("/", AA17)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA17, LEN(AA17) - FIND("/", AA17)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.6333333333333333</v>
       </c>
     </row>
@@ -2114,7 +2090,7 @@
         <v>83</v>
       </c>
       <c r="AB18">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA18,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA18, FIND("/", AA18)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA18, LEN(AA18) - FIND("/", AA18)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.26666666666666666</v>
       </c>
     </row>
@@ -2182,7 +2158,7 @@
         <v>84</v>
       </c>
       <c r="AB19">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA19,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA19, FIND("/", AA19)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA19, LEN(AA19) - FIND("/", AA19)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2244,7 +2220,7 @@
         <v>85</v>
       </c>
       <c r="AB20">
-        <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA20,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA20, FIND("/", AA20)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA20, LEN(AA20) - FIND("/", AA20)),ratings,0)))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.48333333333333328</v>
       </c>
     </row>
@@ -4175,7 +4151,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E31">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>OR(ISBLANK(F3), NOT(F3))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4192,7 +4168,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:V17">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(links, R3) &gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
working through a pitch - again. Removed strategy as a stat, should have done this way, way sooner.
</commit_message>
<xml_diff>
--- a/plans/stats wiggler.xlsx
+++ b/plans/stats wiggler.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D6702-9566-4386-88E1-318278AE4DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11550"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -33,17 +34,26 @@
     <definedName name="weights" localSheetId="0">'Sheet1 (2)'!$I$3:$I$32</definedName>
     <definedName name="weights">Sheet1!$I$3:$I$31</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="90">
   <si>
     <t>BATTING</t>
   </si>
@@ -207,9 +217,6 @@
     <t>pos</t>
   </si>
   <si>
-    <t>strategy</t>
-  </si>
-  <si>
     <t>leadership</t>
   </si>
   <si>
@@ -237,9 +244,6 @@
     <t>defense</t>
   </si>
   <si>
-    <t>edge</t>
-  </si>
-  <si>
     <t>pitching</t>
   </si>
   <si>
@@ -316,13 +320,16 @@
   </si>
   <si>
     <t>Discipline/Trickery</t>
+  </si>
+  <si>
+    <t>remove links?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +338,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -502,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -520,7 +543,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -831,12 +855,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="C16:D17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,20 +908,18 @@
       <c r="U1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="X1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="W1" s="17"/>
+      <c r="X1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -938,23 +960,20 @@
         <f t="array" aca="1" ref="U2" ca="1">SUM(IF(attribs=U1,adjusted,0))</f>
         <v>2.6619047619047618</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="X2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="Y2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="17" t="s">
         <v>5</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -1036,23 +1055,20 @@
         <f t="array" ref="U3">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
         <v>discipline</v>
       </c>
-      <c r="W3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="W3" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="Y3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AA3" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -1119,23 +1135,20 @@
         <f t="array" ref="U4">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
         <v>timing</v>
       </c>
-      <c r="W4" t="s">
-        <v>63</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="W4" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="X4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA4" s="17" t="s">
+      <c r="Z4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA4" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="AB4" s="17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -1202,23 +1215,20 @@
         <f t="array" ref="U5">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
         <v>calling</v>
       </c>
-      <c r="W5" t="s">
-        <v>65</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="W5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="X5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="Y5" s="17" t="s">
+      <c r="Y5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="17" t="s">
+      <c r="Z5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="AA5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>6</v>
+      <c r="AA5" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1285,24 +1295,6 @@
         <f t="array" ref="U6">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
         <v>awareness</v>
       </c>
-      <c r="W6" t="s">
-        <v>64</v>
-      </c>
-      <c r="X6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z6" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1435,7 +1427,7 @@
       </c>
       <c r="U8" s="11" t="str">
         <f t="array" ref="U8">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>strategy</v>
+        <v>sparkle</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1447,12 +1439,10 @@
       <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G9" s="8">
         <f t="array" ref="G9">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -1505,20 +1495,20 @@
         <v>recovery</v>
       </c>
       <c r="W9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="X9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y9">
         <f t="shared" ref="Y9:Y16" ca="1" si="2">IFERROR(INDEX(adjusted,MATCH(X9,ratings,0)), INDEX(adjusted,MATCH(LEFT(X9, FIND("/", X9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X9, LEN(X9) - FIND("/", X9)),ratings,0)))</f>
         <v>0.7</v>
       </c>
       <c r="Z9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AB9">
         <f t="shared" ref="AB9:AB20" ca="1" si="3">IFERROR(INDEX(adjusted,MATCH(AA9,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA9, FIND("/", AA9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA9, LEN(AA9) - FIND("/", AA9)),ratings,0)))</f>
@@ -1533,17 +1523,15 @@
         <v>1.5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G10" s="2">
         <f t="array" ref="G10">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -1576,20 +1564,20 @@
         <v>teach</v>
       </c>
       <c r="W10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="X10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Y10">
         <f t="shared" ca="1" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Z10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="3"/>
@@ -1605,14 +1593,12 @@
       <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="5" t="b">
+      <c r="E11" s="14"/>
+      <c r="F11" s="5" t="str">
         <f t="shared" ref="F11" si="4">IF(ISBLANK(E11), "",
     INDEX(attribs, MATCH(E11,ratings,0))=D11
 )</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G11" s="5">
         <f t="array" ref="G11">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -1650,20 +1636,20 @@
         <v/>
       </c>
       <c r="W11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="X11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Z11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="3"/>
@@ -1712,20 +1698,20 @@
         <v/>
       </c>
       <c r="W12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="X12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Y12">
         <f t="shared" ca="1" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Z12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="3"/>
@@ -1741,12 +1727,10 @@
       <c r="D13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="5" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E13" s="14"/>
+      <c r="F13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G13" s="5">
         <f t="array" ref="G13">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -1776,20 +1760,20 @@
         <v/>
       </c>
       <c r="W13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="X13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y13">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="Z13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="3"/>
@@ -1800,7 +1784,7 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>4</v>
@@ -1838,20 +1822,20 @@
         <v/>
       </c>
       <c r="W14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="X14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y14">
         <f t="shared" ca="1" si="2"/>
         <v>0.6333333333333333</v>
       </c>
       <c r="Z14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="3"/>
@@ -1904,20 +1888,20 @@
         <v/>
       </c>
       <c r="W15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="X15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Y15">
         <f t="shared" ca="1" si="2"/>
         <v>0.76666666666666661</v>
       </c>
       <c r="Z15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="3"/>
@@ -1966,20 +1950,20 @@
         <v/>
       </c>
       <c r="W16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="X16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="2"/>
         <v>0.48333333333333328</v>
       </c>
       <c r="Z16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="3"/>
@@ -1995,12 +1979,10 @@
       <c r="D17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E17" s="14"/>
+      <c r="F17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G17" s="5">
         <f t="array" ref="G17">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -2030,10 +2012,10 @@
         <v/>
       </c>
       <c r="Z17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="3"/>
@@ -2074,20 +2056,20 @@
         <v>6</v>
       </c>
       <c r="W18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="X18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y18">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X18,ratings,0)), INDEX(adjusted,MATCH(LEFT(X18, FIND("/", X18)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X18, LEN(X18) - FIND("/", X18)),ratings,0)))</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="Z18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AB18">
         <f t="shared" ca="1" si="3"/>
@@ -2102,17 +2084,15 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G19" s="2">
         <f t="array" ref="G19">MATCH(ROW()-ROW($A$2),sections,1)</f>
@@ -2142,20 +2122,20 @@
         <v/>
       </c>
       <c r="W19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="X19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y19">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X19,ratings,0)), INDEX(adjusted,MATCH(LEFT(X19, FIND("/", X19)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X19, LEN(X19) - FIND("/", X19)),ratings,0)))</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="Z19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AB19">
         <f t="shared" ca="1" si="3"/>
@@ -2166,7 +2146,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>7</v>
@@ -2204,20 +2184,20 @@
         <v/>
       </c>
       <c r="W20" t="s">
+        <v>72</v>
+      </c>
+      <c r="X20" t="s">
         <v>74</v>
-      </c>
-      <c r="X20" t="s">
-        <v>76</v>
       </c>
       <c r="Y20">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X20,ratings,0)), INDEX(adjusted,MATCH(LEFT(X20, FIND("/", X20)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X20, LEN(X20) - FIND("/", X20)),ratings,0)))</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="Z20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB20">
         <f t="shared" ca="1" si="3"/>
@@ -2228,7 +2208,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="14"/>
       <c r="C21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>8</v>
@@ -2266,21 +2246,21 @@
         <v/>
       </c>
       <c r="W21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="X21" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="Y21">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X21,ratings,0)), INDEX(adjusted,MATCH(LEFT(X21, FIND("/", X21)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X21, LEN(X21) - FIND("/", X21)),ratings,0)))</f>
-        <v>0.48333333333333328</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>4</v>
@@ -2318,10 +2298,10 @@
         <v/>
       </c>
       <c r="Z22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB22">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA22,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA22, FIND("/", AA22)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA22, LEN(AA22) - FIND("/", AA22)),ratings,0)))</f>
@@ -2330,7 +2310,7 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2">
         <v>1.5</v>
@@ -2358,10 +2338,10 @@
         <v>1</v>
       </c>
       <c r="Z23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB23">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA23,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA23, FIND("/", AA23)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA23, LEN(AA23) - FIND("/", AA23)),ratings,0)))</f>
@@ -2372,7 +2352,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="14"/>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>8</v>
@@ -2394,10 +2374,10 @@
         <v>0.5</v>
       </c>
       <c r="Z24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA24" t="s">
         <v>74</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>76</v>
       </c>
       <c r="AB24">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA24,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA24, FIND("/", AA24)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA24, LEN(AA24) - FIND("/", AA24)),ratings,0)))</f>
@@ -2429,15 +2409,18 @@
       <c r="I25" s="6">
         <v>1</v>
       </c>
+      <c r="R25" t="s">
+        <v>89</v>
+      </c>
       <c r="Z25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA25" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB25">
+        <v>84</v>
+      </c>
+      <c r="AB25" t="e">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA25,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA25, FIND("/", AA25)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA25, LEN(AA25) - FIND("/", AA25)),ratings,0)))</f>
-        <v>0.48333333333333328</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -2522,7 +2505,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="14"/>
       <c r="C29" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>8</v>
@@ -2574,7 +2557,7 @@
       <c r="A31" s="4"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>9</v>
@@ -2677,7 +2660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V32"/>
   <sheetViews>

</xml_diff>

<commit_message>
kill all the stats
</commit_message>
<xml_diff>
--- a/plans/stats wiggler.xlsx
+++ b/plans/stats wiggler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D6702-9566-4386-88E1-318278AE4DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30E3655-6AD5-4EC4-96FC-93E855E1782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,6 +35,7 @@
     <definedName name="weights">Sheet1!$I$3:$I$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="89">
   <si>
     <t>BATTING</t>
   </si>
@@ -290,9 +291,6 @@
   </si>
   <si>
     <t>Reach</t>
-  </si>
-  <si>
-    <t>Control</t>
   </si>
   <si>
     <t>Grabbiness</t>
@@ -860,7 +858,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,19 +944,19 @@
       </c>
       <c r="R2" s="13">
         <f t="array" aca="1" ref="R2" ca="1">SUM(IF(attribs=R1,adjusted,0))</f>
-        <v>2.3507936507936509</v>
+        <v>2.4047619047619047</v>
       </c>
       <c r="S2" s="13">
         <f t="array" aca="1" ref="S2" ca="1">SUM(IF(attribs=S1,adjusted,0))</f>
-        <v>2.3698412698412703</v>
+        <v>2.6190476190476195</v>
       </c>
       <c r="T2" s="13">
         <f t="array" aca="1" ref="T2" ca="1">SUM(IF(attribs=T1,adjusted,0))</f>
-        <v>2.617460317460317</v>
+        <v>2.5714285714285712</v>
       </c>
       <c r="U2" s="13">
         <f t="array" aca="1" ref="U2" ca="1">SUM(IF(attribs=U1,adjusted,0))</f>
-        <v>2.6619047619047618</v>
+        <v>2.4047619047619047</v>
       </c>
       <c r="W2" s="17" t="s">
         <v>64</v>
@@ -1010,7 +1008,7 @@
     INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)+1)-(INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1))),
     1
 ))</f>
-        <v>0.53333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1033,11 +1031,11 @@
       </c>
       <c r="O3" t="str">
         <f t="array" aca="1" ref="O3" ca="1">IF(SUM(IF(OFFSET(attribs,INDEX(sections, ROW()-ROW($A$2))-1, 0, INDEX(sections, ROW()-ROW($A$2)+1) - INDEX(sections, ROW()-ROW($A$2)))=U$1,1,0))&gt;0, "", INDEX(toplevel,INDEX(sections,ROW()-ROW($A$2))))</f>
-        <v/>
+        <v>BATTING</v>
       </c>
       <c r="P3" t="str">
         <f t="array" aca="1" ref="P3" ca="1">IF(SUM(IF(OFFSET(attribs,INDEX(sections, ROW()-ROW($A$2))-1, 0, INDEX(sections, ROW()-ROW($A$2)+1) - INDEX(sections, ROW()-ROW($A$2)))=V$1,1,0))&gt;0, "", INDEX(toplevel,INDEX(sections,ROW()-ROW($A$2))))</f>
-        <v>BATTING</v>
+        <v/>
       </c>
       <c r="R3" s="11" t="str">
         <f t="array" ref="R3">IFERROR(INDEX(ratings,SMALL(IF(attribs=R$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(R$2))), "")</f>
@@ -1049,11 +1047,11 @@
       </c>
       <c r="T3" s="10" t="str">
         <f t="array" ref="T3">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>control</v>
+        <v>discipline</v>
       </c>
       <c r="U3" s="10" t="str">
         <f t="array" ref="U3">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>discipline</v>
+        <v>timing</v>
       </c>
       <c r="W3" s="17" t="s">
         <v>65</v>
@@ -1091,7 +1089,7 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I4" s="6">
         <v>3</v>
@@ -1129,11 +1127,11 @@
       </c>
       <c r="T4" s="11" t="str">
         <f t="array" ref="T4">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>throwing</v>
+        <v>grabbiness</v>
       </c>
       <c r="U4" s="11" t="str">
         <f t="array" ref="U4">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>timing</v>
+        <v>calling</v>
       </c>
       <c r="W4" s="17" t="s">
         <v>62</v>
@@ -1154,12 +1152,8 @@
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1171,10 +1165,10 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I5" s="6">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>8</v>
@@ -1197,7 +1191,7 @@
       </c>
       <c r="P5" t="str">
         <f t="array" aca="1" ref="P5" ca="1">IF(SUM(IF(OFFSET(attribs,INDEX(sections, ROW()-ROW($A$2))-1, 0, INDEX(sections, ROW()-ROW($A$2)+1) - INDEX(sections, ROW()-ROW($A$2)))=V$1,1,0))&gt;0, "", INDEX(toplevel,INDEX(sections,ROW()-ROW($A$2))))</f>
-        <v>DEFENSE</v>
+        <v/>
       </c>
       <c r="R5" s="11" t="str">
         <f t="array" ref="R5">IFERROR(INDEX(ratings,SMALL(IF(attribs=R$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(R$2))), "")</f>
@@ -1209,11 +1203,11 @@
       </c>
       <c r="T5" s="11" t="str">
         <f t="array" ref="T5">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>grabbiness</v>
+        <v>accuracy</v>
       </c>
       <c r="U5" s="11" t="str">
         <f t="array" ref="U5">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>calling</v>
+        <v>trickery</v>
       </c>
       <c r="W5" s="17" t="s">
         <v>63</v>
@@ -1238,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
@@ -1251,7 +1245,7 @@
       </c>
       <c r="H6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I6" s="9">
         <v>1</v>
@@ -1289,11 +1283,11 @@
       </c>
       <c r="T6" s="11" t="str">
         <f t="array" ref="T6">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>accuracy</v>
+        <v>I.T.</v>
       </c>
       <c r="U6" s="11" t="str">
         <f t="array" ref="U6">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>awareness</v>
+        <v>sparkle</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1358,11 +1352,11 @@
       </c>
       <c r="T7" s="11" t="str">
         <f t="array" ref="T7">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>I.T.</v>
+        <v>positivity</v>
       </c>
       <c r="U7" s="11" t="str">
         <f t="array" ref="U7">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>trickery</v>
+        <v>recovery</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1423,11 +1417,11 @@
       </c>
       <c r="T8" s="11" t="str">
         <f t="array" ref="T8">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>positivity</v>
+        <v>support</v>
       </c>
       <c r="U8" s="11" t="str">
         <f t="array" ref="U8">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>sparkle</v>
+        <v>teach</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1488,21 +1482,21 @@
       </c>
       <c r="T9" s="11" t="str">
         <f t="array" ref="T9">IFERROR(INDEX(ratings,SMALL(IF(attribs=T$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(T$2))), "")</f>
-        <v>support</v>
+        <v/>
       </c>
       <c r="U9" s="11" t="str">
         <f t="array" ref="U9">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>recovery</v>
+        <v/>
       </c>
       <c r="W9" t="s">
         <v>70</v>
       </c>
       <c r="X9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Y9">
         <f t="shared" ref="Y9:Y16" ca="1" si="2">IFERROR(INDEX(adjusted,MATCH(X9,ratings,0)), INDEX(adjusted,MATCH(LEFT(X9, FIND("/", X9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X9, LEN(X9) - FIND("/", X9)),ratings,0)))</f>
-        <v>0.7</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="Z9" t="s">
         <v>70</v>
@@ -1512,7 +1506,7 @@
       </c>
       <c r="AB9">
         <f t="shared" ref="AB9:AB20" ca="1" si="3">IFERROR(INDEX(adjusted,MATCH(AA9,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA9, FIND("/", AA9)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA9, LEN(AA9) - FIND("/", AA9)),ratings,0)))</f>
-        <v>0.53333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1539,7 +1533,7 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="I10" s="3">
         <v>0.5</v>
@@ -1561,7 +1555,7 @@
       </c>
       <c r="U10" s="11" t="str">
         <f t="array" ref="U10">IFERROR(INDEX(ratings,SMALL(IF(attribs=U$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(U$2))), "")</f>
-        <v>teach</v>
+        <v/>
       </c>
       <c r="W10" t="s">
         <v>70</v>
@@ -1587,15 +1581,11 @@
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>9</v>
-      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="5" t="str">
-        <f t="shared" ref="F11" si="4">IF(ISBLANK(E11), "",
+        <f>IF(ISBLANK(E11), "",
     INDEX(attribs, MATCH(E11,ratings,0))=D11
 )</f>
         <v/>
@@ -1605,7 +1595,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ref="H11" ca="1" si="5">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
+        <f ca="1">INDEX(toplevelws,INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)))*
 I11/
 SUM(OFFSET(
     weights,
@@ -1614,10 +1604,10 @@
     INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1)+1)-(INDEX(sections,MATCH(ROW()-ROW($A$2),sections,1))),
     1
 ))</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I11" s="6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R11" s="11" t="str">
         <f t="array" ref="R11">IFERROR(INDEX(ratings,SMALL(IF(attribs=R$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(R$2))), "")</f>
@@ -1643,7 +1633,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="s">
         <v>70</v>
@@ -1676,7 +1666,7 @@
       </c>
       <c r="H12" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I12" s="6">
         <v>1</v>
@@ -1701,11 +1691,11 @@
         <v>71</v>
       </c>
       <c r="X12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Y12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="Z12" t="s">
         <v>71</v>
@@ -1715,18 +1705,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>4</v>
-      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1738,10 +1724,10 @@
       </c>
       <c r="H13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="11" t="str">
         <f t="array" ref="R13">IFERROR(INDEX(ratings,SMALL(IF(attribs=R$1,ROW(attribs)-ROW(INDEX(attribs,1,1))+1),ROW()-ROW(R$2))), "")</f>
@@ -1763,11 +1749,11 @@
         <v>72</v>
       </c>
       <c r="X13" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y13">
+        <v>86</v>
+      </c>
+      <c r="Y13" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="Z13" t="s">
         <v>71</v>
@@ -1800,7 +1786,7 @@
       </c>
       <c r="H14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="I14" s="9">
         <v>2</v>
@@ -1827,9 +1813,9 @@
       <c r="X14" t="s">
         <v>69</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>0.6333333333333333</v>
+        <v>#N/A</v>
       </c>
       <c r="Z14" t="s">
         <v>71</v>
@@ -1839,7 +1825,7 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -1891,21 +1877,11 @@
         <v>73</v>
       </c>
       <c r="X15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76666666666666661</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB15">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.4</v>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1953,21 +1929,21 @@
         <v>73</v>
       </c>
       <c r="X16" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y16">
+        <v>82</v>
+      </c>
+      <c r="Y16" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>0.48333333333333328</v>
+        <v>#N/A</v>
       </c>
       <c r="Z16" t="s">
         <v>72</v>
       </c>
       <c r="AA16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -2017,9 +1993,9 @@
       <c r="AA17" t="s">
         <v>69</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6333333333333333</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -2063,17 +2039,17 @@
       </c>
       <c r="Y18">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X18,ratings,0)), INDEX(adjusted,MATCH(LEFT(X18, FIND("/", X18)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X18, LEN(X18) - FIND("/", X18)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="Z18" t="s">
         <v>73</v>
       </c>
       <c r="AA18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -2100,7 +2076,7 @@
       </c>
       <c r="H19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I19" s="3">
         <v>1.5</v>
@@ -2119,7 +2095,7 @@
       </c>
       <c r="U19" s="10" t="str">
         <f t="array" aca="1" ref="U19:U22" ca="1">IFERROR(INDEX(O$3:O$9,SMALL(IF(O$3:O$9&lt;&gt;"",ROW(O$3:O$9)-ROW(O$2)),ROW()-ROW(U$18))), "")</f>
-        <v/>
+        <v>BATTING</v>
       </c>
       <c r="W19" t="s">
         <v>71</v>
@@ -2129,13 +2105,13 @@
       </c>
       <c r="Y19">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X19,ratings,0)), INDEX(adjusted,MATCH(LEFT(X19, FIND("/", X19)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X19, LEN(X19) - FIND("/", X19)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="Z19" t="s">
         <v>73</v>
       </c>
       <c r="AA19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB19">
         <f t="shared" ca="1" si="3"/>
@@ -2162,10 +2138,10 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I20" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R20" s="11" t="str">
         <f ca="1"/>
@@ -2191,17 +2167,17 @@
       </c>
       <c r="Y20">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X20,ratings,0)), INDEX(adjusted,MATCH(LEFT(X20, FIND("/", X20)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X20, LEN(X20) - FIND("/", X20)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="Z20" t="s">
         <v>73</v>
       </c>
       <c r="AA20" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB20">
+        <v>82</v>
+      </c>
+      <c r="AB20" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48333333333333328</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -2224,10 +2200,10 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I21" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R21" s="11" t="str">
         <f ca="1"/>
@@ -2253,7 +2229,7 @@
       </c>
       <c r="Y21">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(X21,ratings,0)), INDEX(adjusted,MATCH(LEFT(X21, FIND("/", X21)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(X21, LEN(X21) - FIND("/", X21)),ratings,0)))</f>
-        <v>0.33333333333333331</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -2276,7 +2252,7 @@
       </c>
       <c r="H22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22222222222222221</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I22" s="9">
         <v>1</v>
@@ -2305,7 +2281,7 @@
       </c>
       <c r="AB22">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA22,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA22, FIND("/", AA22)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA22, LEN(AA22) - FIND("/", AA22)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2345,7 +2321,7 @@
       </c>
       <c r="AB23">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA23,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA23, FIND("/", AA23)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA23, LEN(AA23) - FIND("/", AA23)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -2381,7 +2357,7 @@
       </c>
       <c r="AB24">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA24,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA24, FIND("/", AA24)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA24, LEN(AA24) - FIND("/", AA24)),ratings,0)))</f>
-        <v>0.22222222222222221</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -2410,13 +2386,13 @@
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z25" t="s">
         <v>73</v>
       </c>
       <c r="AA25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB25" t="e">
         <f ca="1">IFERROR(INDEX(adjusted,MATCH(AA25,ratings,0)), INDEX(adjusted,MATCH(LEFT(AA25, FIND("/", AA25)-1),ratings,0)) + INDEX(adjusted,MATCH(RIGHT(AA25, LEN(AA25) - FIND("/", AA25)),ratings,0)))</f>

</xml_diff>

<commit_message>
pitching target position might finally be solved?
</commit_message>
<xml_diff>
--- a/plans/stats wiggler.xlsx
+++ b/plans/stats wiggler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30E3655-6AD5-4EC4-96FC-93E855E1782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AA2552-E151-44E2-B479-5FE8422DF2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,7 +858,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>